<commit_message>
mengganti totale dengan rumus excel
</commit_message>
<xml_diff>
--- a/app/production/compatibility_model/dashboard/result/export/data_hasil/b450_2022-09-08.xlsx
+++ b/app/production/compatibility_model/dashboard/result/export/data_hasil/b450_2022-09-08.xlsx
@@ -1206,15 +1206,19 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4">
+        <f>SUM(D6:D36)</f>
         <v>2685</v>
       </c>
       <c r="E37" s="4">
+        <f>SUM(E6:E36)</f>
         <v>534</v>
       </c>
       <c r="F37" s="4">
+        <f>SUM(F6:F36)</f>
         <v>-2151</v>
       </c>
       <c r="G37" s="4">
+        <f>E37-D37</f>
         <v>-2151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mengganti progress dengan rumus excel
</commit_message>
<xml_diff>
--- a/app/production/compatibility_model/dashboard/result/export/data_hasil/b450_2022-09-08.xlsx
+++ b/app/production/compatibility_model/dashboard/result/export/data_hasil/b450_2022-09-08.xlsx
@@ -575,9 +575,11 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
+        <f>E6-D6</f>
         <v>-115</v>
       </c>
       <c r="G6" s="1">
+        <f>G5+E6</f>
         <v>-2685</v>
       </c>
     </row>
@@ -596,9 +598,11 @@
         <v>137</v>
       </c>
       <c r="F7" s="1">
+        <f>E7-D7</f>
         <v>-13</v>
       </c>
       <c r="G7" s="1">
+        <f>G6+E7</f>
         <v>-2548</v>
       </c>
     </row>
@@ -617,9 +621,11 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
+        <f>E8-D8</f>
         <v>0</v>
       </c>
       <c r="G8" s="2">
+        <f>G7+E8</f>
         <v>-2548</v>
       </c>
     </row>
@@ -638,9 +644,11 @@
         <v>0</v>
       </c>
       <c r="F9" s="2">
+        <f>E9-D9</f>
         <v>0</v>
       </c>
       <c r="G9" s="2">
+        <f>G8+E9</f>
         <v>-2548</v>
       </c>
     </row>
@@ -659,9 +667,11 @@
         <v>140</v>
       </c>
       <c r="F10" s="1">
+        <f>E10-D10</f>
         <v>-10</v>
       </c>
       <c r="G10" s="1">
+        <f>G9+E10</f>
         <v>-2408</v>
       </c>
     </row>
@@ -680,9 +690,11 @@
         <v>137</v>
       </c>
       <c r="F11" s="1">
+        <f>E11-D11</f>
         <v>22</v>
       </c>
       <c r="G11" s="1">
+        <f>G10+E11</f>
         <v>-2271</v>
       </c>
     </row>
@@ -701,9 +713,11 @@
         <v>10</v>
       </c>
       <c r="F12" s="1">
+        <f>E12-D12</f>
         <v>-140</v>
       </c>
       <c r="G12" s="1">
+        <f>G11+E12</f>
         <v>-2261</v>
       </c>
     </row>
@@ -722,9 +736,11 @@
         <v>110</v>
       </c>
       <c r="F13" s="1">
+        <f>E13-D13</f>
         <v>-5</v>
       </c>
       <c r="G13" s="1">
+        <f>G12+E13</f>
         <v>-2151</v>
       </c>
     </row>
@@ -743,9 +759,11 @@
         <v>0</v>
       </c>
       <c r="F14" s="1">
+        <f>E14-D14</f>
         <v>-150</v>
       </c>
       <c r="G14" s="1">
+        <f>G13+E14</f>
         <v>-2151</v>
       </c>
     </row>
@@ -764,9 +782,11 @@
         <v>0</v>
       </c>
       <c r="F15" s="2">
+        <f>E15-D15</f>
         <v>0</v>
       </c>
       <c r="G15" s="2">
+        <f>G14+E15</f>
         <v>-2151</v>
       </c>
     </row>
@@ -785,9 +805,11 @@
         <v>0</v>
       </c>
       <c r="F16" s="2">
+        <f>E16-D16</f>
         <v>0</v>
       </c>
       <c r="G16" s="2">
+        <f>G15+E16</f>
         <v>-2151</v>
       </c>
     </row>
@@ -806,9 +828,11 @@
         <v>0</v>
       </c>
       <c r="F17" s="1">
+        <f>E17-D17</f>
         <v>-150</v>
       </c>
       <c r="G17" s="1">
+        <f>G16+E17</f>
         <v>-2151</v>
       </c>
     </row>
@@ -827,9 +851,11 @@
         <v>0</v>
       </c>
       <c r="F18" s="1">
+        <f>E18-D18</f>
         <v>-115</v>
       </c>
       <c r="G18" s="1">
+        <f>G17+E18</f>
         <v>-2151</v>
       </c>
     </row>
@@ -848,9 +874,11 @@
         <v>0</v>
       </c>
       <c r="F19" s="1">
+        <f>E19-D19</f>
         <v>-150</v>
       </c>
       <c r="G19" s="1">
+        <f>G18+E19</f>
         <v>-2151</v>
       </c>
     </row>
@@ -869,9 +897,11 @@
         <v>0</v>
       </c>
       <c r="F20" s="1">
+        <f>E20-D20</f>
         <v>-115</v>
       </c>
       <c r="G20" s="1">
+        <f>G19+E20</f>
         <v>-2151</v>
       </c>
     </row>
@@ -890,9 +920,11 @@
         <v>0</v>
       </c>
       <c r="F21" s="1">
+        <f>E21-D21</f>
         <v>-150</v>
       </c>
       <c r="G21" s="1">
+        <f>G20+E21</f>
         <v>-2151</v>
       </c>
     </row>
@@ -911,9 +943,11 @@
         <v>0</v>
       </c>
       <c r="F22" s="2">
+        <f>E22-D22</f>
         <v>0</v>
       </c>
       <c r="G22" s="2">
+        <f>G21+E22</f>
         <v>-2151</v>
       </c>
     </row>
@@ -932,9 +966,11 @@
         <v>0</v>
       </c>
       <c r="F23" s="2">
+        <f>E23-D23</f>
         <v>0</v>
       </c>
       <c r="G23" s="2">
+        <f>G22+E23</f>
         <v>-2151</v>
       </c>
     </row>
@@ -953,9 +989,11 @@
         <v>0</v>
       </c>
       <c r="F24" s="1">
+        <f>E24-D24</f>
         <v>-150</v>
       </c>
       <c r="G24" s="1">
+        <f>G23+E24</f>
         <v>-2151</v>
       </c>
     </row>
@@ -974,9 +1012,11 @@
         <v>0</v>
       </c>
       <c r="F25" s="1">
+        <f>E25-D25</f>
         <v>-115</v>
       </c>
       <c r="G25" s="1">
+        <f>G24+E25</f>
         <v>-2151</v>
       </c>
     </row>
@@ -995,9 +1035,11 @@
         <v>0</v>
       </c>
       <c r="F26" s="1">
+        <f>E26-D26</f>
         <v>-150</v>
       </c>
       <c r="G26" s="1">
+        <f>G25+E26</f>
         <v>-2151</v>
       </c>
     </row>
@@ -1016,9 +1058,11 @@
         <v>0</v>
       </c>
       <c r="F27" s="1">
+        <f>E27-D27</f>
         <v>-115</v>
       </c>
       <c r="G27" s="1">
+        <f>G26+E27</f>
         <v>-2151</v>
       </c>
     </row>
@@ -1037,9 +1081,11 @@
         <v>0</v>
       </c>
       <c r="F28" s="1">
+        <f>E28-D28</f>
         <v>-150</v>
       </c>
       <c r="G28" s="1">
+        <f>G27+E28</f>
         <v>-2151</v>
       </c>
     </row>
@@ -1058,9 +1104,11 @@
         <v>0</v>
       </c>
       <c r="F29" s="2">
+        <f>E29-D29</f>
         <v>0</v>
       </c>
       <c r="G29" s="2">
+        <f>G28+E29</f>
         <v>-2151</v>
       </c>
     </row>
@@ -1079,9 +1127,11 @@
         <v>0</v>
       </c>
       <c r="F30" s="2">
+        <f>E30-D30</f>
         <v>0</v>
       </c>
       <c r="G30" s="2">
+        <f>G29+E30</f>
         <v>-2151</v>
       </c>
     </row>
@@ -1100,9 +1150,11 @@
         <v>0</v>
       </c>
       <c r="F31" s="1">
+        <f>E31-D31</f>
         <v>-150</v>
       </c>
       <c r="G31" s="1">
+        <f>G30+E31</f>
         <v>-2151</v>
       </c>
     </row>
@@ -1121,9 +1173,11 @@
         <v>0</v>
       </c>
       <c r="F32" s="1">
+        <f>E32-D32</f>
         <v>-115</v>
       </c>
       <c r="G32" s="1">
+        <f>G31+E32</f>
         <v>-2151</v>
       </c>
     </row>
@@ -1142,9 +1196,11 @@
         <v>0</v>
       </c>
       <c r="F33" s="1">
+        <f>E33-D33</f>
         <v>-115</v>
       </c>
       <c r="G33" s="1">
+        <f>G32+E33</f>
         <v>-2151</v>
       </c>
     </row>
@@ -1163,9 +1219,11 @@
         <v>0</v>
       </c>
       <c r="F34" s="1">
+        <f>E34-D34</f>
         <v>0</v>
       </c>
       <c r="G34" s="1">
+        <f>G33+E34</f>
         <v>-2151</v>
       </c>
     </row>
@@ -1184,9 +1242,11 @@
         <v>0</v>
       </c>
       <c r="F35" s="1">
+        <f>E35-D35</f>
         <v>0</v>
       </c>
       <c r="G35" s="1">
+        <f>G34+E35</f>
         <v>-2151</v>
       </c>
     </row>

</xml_diff>